<commit_message>
update july, 14 2022
</commit_message>
<xml_diff>
--- a/public/assets/template/import_prk_template.xlsx
+++ b/public/assets/template/import_prk_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\pln-laravel\public\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FD2AC10-012A-424F-99F8-1ADD43966B59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C69F71F-007B-45EF-B985-8C144BEE96F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3B700C8B-DF7B-4FF2-AADC-B9758107657C}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nama Project</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Basket</t>
+  </si>
+  <si>
+    <t>RP Jasa</t>
   </si>
 </sst>
 </file>
@@ -447,18 +450,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0055F1BE-D36D-4900-BAE7-AAE317A6DB22}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,6 +477,9 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>